<commit_message>
Run co-sim on ieee39
</commit_message>
<xml_diff>
--- a/jwang/case/ieee39_ev2.xlsx
+++ b/jwang/case/ieee39_ev2.xlsx
@@ -2236,7 +2236,7 @@
         <v>0.05</v>
       </c>
       <c r="I2" t="str">
-        <v>1.01</v>
+        <v>5</v>
       </c>
       <c r="J2" t="str">
         <v>0.1</v>
@@ -2277,7 +2277,7 @@
         <v>0.05</v>
       </c>
       <c r="I3" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J3" t="str">
         <v>0.1</v>
@@ -2318,7 +2318,7 @@
         <v>0.05</v>
       </c>
       <c r="I4" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J4" t="str">
         <v>0.1</v>
@@ -2359,7 +2359,7 @@
         <v>0.05</v>
       </c>
       <c r="I5" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J5" t="str">
         <v>0.1</v>
@@ -2400,7 +2400,7 @@
         <v>0.05</v>
       </c>
       <c r="I6" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J6" t="str">
         <v>0.1</v>
@@ -2441,7 +2441,7 @@
         <v>0.05</v>
       </c>
       <c r="I7" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J7" t="str">
         <v>0.1</v>
@@ -2482,7 +2482,7 @@
         <v>0.05</v>
       </c>
       <c r="I8" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J8" t="str">
         <v>0.1</v>
@@ -2523,7 +2523,7 @@
         <v>0.05</v>
       </c>
       <c r="I9" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J9" t="str">
         <v>0.1</v>
@@ -2564,7 +2564,7 @@
         <v>0.05</v>
       </c>
       <c r="I10" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J10" t="str">
         <v>0.1</v>
@@ -2605,7 +2605,7 @@
         <v>0.05</v>
       </c>
       <c r="I11" t="str">
-        <v>1.05</v>
+        <v>5</v>
       </c>
       <c r="J11" t="str">
         <v>0.1</v>
@@ -5428,7 +5428,7 @@
         <v>1.4</v>
       </c>
       <c r="K2" t="str">
-        <v>10.4</v>
+        <v>12</v>
       </c>
       <c r="L2" t="str">
         <v>0.1</v>
@@ -5484,7 +5484,7 @@
         <v>3</v>
       </c>
       <c r="K3" t="str">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="L3" t="str">
         <v>0.1</v>
@@ -5540,7 +5540,7 @@
         <v>3</v>
       </c>
       <c r="K4" t="str">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="L4" t="str">
         <v>0.1</v>
@@ -5596,7 +5596,7 @@
         <v>1.5806</v>
       </c>
       <c r="K5" t="str">
-        <v>6.82</v>
+        <v>8</v>
       </c>
       <c r="L5" t="str">
         <v>0.1</v>
@@ -5652,7 +5652,7 @@
         <v>1.5854</v>
       </c>
       <c r="K6" t="str">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="L6" t="str">
         <v>0.1</v>
@@ -5708,7 +5708,7 @@
         <v>2.5777</v>
       </c>
       <c r="K7" t="str">
-        <v>6.97</v>
+        <v>7</v>
       </c>
       <c r="L7" t="str">
         <v>0.1</v>
@@ -5764,7 +5764,7 @@
         <v>0.7876</v>
       </c>
       <c r="K8" t="str">
-        <v>5.95</v>
+        <v>7</v>
       </c>
       <c r="L8" t="str">
         <v>0.1</v>
@@ -5820,7 +5820,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="str">
-        <v>5.64</v>
+        <v>7</v>
       </c>
       <c r="L9" t="str">
         <v>0.1</v>
@@ -5876,7 +5876,7 @@
         <v>1.428</v>
       </c>
       <c r="K10" t="str">
-        <v>8.65</v>
+        <v>10</v>
       </c>
       <c r="L10" t="str">
         <v>0.1</v>
@@ -6349,10 +6349,10 @@
         <v>0.5617</v>
       </c>
       <c r="K2" t="str">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L2" t="str">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="M2" t="str">
         <v>5.7485</v>

</xml_diff>

<commit_message>
Fix runopp_map, use DCOPF if ACOPF failed
</commit_message>
<xml_diff>
--- a/jwang/case/ieee39_ev2.xlsx
+++ b/jwang/case/ieee39_ev2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/jwang/case/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4978F232-899A-7347-8C2B-3E7095999550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD51633-007D-1C43-BD83-292F34BA44D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3213" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3174" uniqueCount="753">
   <si>
     <t>uid</t>
   </si>
@@ -4476,7 +4476,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4550,11 +4550,11 @@
       <c r="H2" t="s">
         <v>642</v>
       </c>
-      <c r="I2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>245</v>
+      <c r="I2" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
       </c>
       <c r="K2" t="s">
         <v>642</v>
@@ -4594,11 +4594,11 @@
       <c r="H3" t="s">
         <v>642</v>
       </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" t="s">
-        <v>245</v>
+      <c r="I3" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3" t="s">
         <v>642</v>
@@ -4638,11 +4638,11 @@
       <c r="H4" t="s">
         <v>642</v>
       </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>245</v>
+      <c r="I4" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
       </c>
       <c r="K4" t="s">
         <v>642</v>
@@ -4682,11 +4682,11 @@
       <c r="H5" t="s">
         <v>642</v>
       </c>
-      <c r="I5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>245</v>
+      <c r="I5" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>642</v>
@@ -4726,11 +4726,11 @@
       <c r="H6" t="s">
         <v>642</v>
       </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>245</v>
+      <c r="I6" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
       <c r="K6" t="s">
         <v>642</v>
@@ -4770,11 +4770,11 @@
       <c r="H7" t="s">
         <v>642</v>
       </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" t="s">
-        <v>245</v>
+      <c r="I7" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
       </c>
       <c r="K7" t="s">
         <v>642</v>
@@ -4814,11 +4814,11 @@
       <c r="H8" t="s">
         <v>642</v>
       </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" t="s">
-        <v>245</v>
+      <c r="I8" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
       </c>
       <c r="K8" t="s">
         <v>642</v>
@@ -4858,11 +4858,11 @@
       <c r="H9" t="s">
         <v>642</v>
       </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" t="s">
-        <v>245</v>
+      <c r="I9" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
       </c>
       <c r="K9" t="s">
         <v>642</v>
@@ -4902,11 +4902,11 @@
       <c r="H10" t="s">
         <v>642</v>
       </c>
-      <c r="I10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" t="s">
-        <v>245</v>
+      <c r="I10" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="K10" t="s">
         <v>642</v>
@@ -4946,11 +4946,11 @@
       <c r="H11" t="s">
         <v>642</v>
       </c>
-      <c r="I11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" t="s">
-        <v>245</v>
+      <c r="I11" s="2">
+        <v>1.05</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
       </c>
       <c r="K11" t="s">
         <v>642</v>
@@ -4968,7 +4968,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:N1 A2:E11 G2:N11" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:N1 A2:E11 G2:H11 K3:N11 K2:N2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -7694,7 +7694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -7785,11 +7787,11 @@
       <c r="J2" t="s">
         <v>244</v>
       </c>
-      <c r="K2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" t="s">
-        <v>245</v>
+      <c r="K2" s="2">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
       </c>
       <c r="M2" t="s">
         <v>246</v>
@@ -7841,11 +7843,11 @@
       <c r="J3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" t="s">
-        <v>245</v>
+      <c r="K3" s="2">
+        <v>7</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
       </c>
       <c r="M3" t="s">
         <v>255</v>
@@ -7897,11 +7899,11 @@
       <c r="J4" t="s">
         <v>26</v>
       </c>
-      <c r="K4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" t="s">
-        <v>245</v>
+      <c r="K4" s="2">
+        <v>8</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
       </c>
       <c r="M4" t="s">
         <v>263</v>
@@ -7953,11 +7955,11 @@
       <c r="J5" t="s">
         <v>271</v>
       </c>
-      <c r="K5" t="s">
-        <v>54</v>
-      </c>
-      <c r="L5" t="s">
-        <v>245</v>
+      <c r="K5" s="2">
+        <v>7</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
       </c>
       <c r="M5" t="s">
         <v>272</v>
@@ -8009,11 +8011,11 @@
       <c r="J6" t="s">
         <v>280</v>
       </c>
-      <c r="K6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" t="s">
-        <v>245</v>
+      <c r="K6" s="2">
+        <v>7</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
       </c>
       <c r="M6" t="s">
         <v>281</v>
@@ -8065,11 +8067,11 @@
       <c r="J7" t="s">
         <v>288</v>
       </c>
-      <c r="K7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" t="s">
-        <v>245</v>
+      <c r="K7" s="2">
+        <v>8</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
       </c>
       <c r="M7" t="s">
         <v>289</v>
@@ -8121,11 +8123,11 @@
       <c r="J8" t="s">
         <v>297</v>
       </c>
-      <c r="K8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L8" t="s">
-        <v>245</v>
+      <c r="K8" s="2">
+        <v>7</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
       </c>
       <c r="M8" t="s">
         <v>298</v>
@@ -8177,11 +8179,11 @@
       <c r="J9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9" t="s">
-        <v>245</v>
+      <c r="K9" s="2">
+        <v>7</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
       </c>
       <c r="M9" t="s">
         <v>305</v>
@@ -8233,11 +8235,11 @@
       <c r="J10" t="s">
         <v>313</v>
       </c>
-      <c r="K10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" t="s">
-        <v>245</v>
+      <c r="K10" s="2">
+        <v>10</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
       </c>
       <c r="M10" t="s">
         <v>314</v>
@@ -8320,7 +8322,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:S11" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:S1 A11:S11 A2:J10 M2:S10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8616,7 +8618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -8710,8 +8714,8 @@
       <c r="J2" t="s">
         <v>380</v>
       </c>
-      <c r="K2" t="s">
-        <v>95</v>
+      <c r="K2" s="2">
+        <v>15</v>
       </c>
       <c r="L2" t="s">
         <v>26</v>
@@ -8744,7 +8748,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:T2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:T1 A2:J2 L2:T2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8865,7 +8869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Run cosim, save ev data
</commit_message>
<xml_diff>
--- a/jwang/case/ieee39_ev2.xlsx
+++ b/jwang/case/ieee39_ev2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang175\.ssh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36B9E8D-6B80-4A15-ABC4-AC24E89A1243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453470DD-850A-48E9-9658-D6384E6BD161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3305" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3293" uniqueCount="771">
   <si>
     <t>uid</t>
   </si>
@@ -2740,9 +2740,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>115</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>123</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>131</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>152</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>170</v>
       </c>
@@ -4514,11 +4514,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4562,7 +4564,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -4593,8 +4595,8 @@
       <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" t="s">
-        <v>627</v>
+      <c r="K2">
+        <v>0.8</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
@@ -4606,7 +4608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4637,8 +4639,8 @@
       <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" t="s">
-        <v>627</v>
+      <c r="K3">
+        <v>0.8</v>
       </c>
       <c r="L3" t="s">
         <v>15</v>
@@ -4650,7 +4652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -4681,8 +4683,8 @@
       <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" t="s">
-        <v>627</v>
+      <c r="K4">
+        <v>0.8</v>
       </c>
       <c r="L4" t="s">
         <v>15</v>
@@ -4694,7 +4696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -4725,8 +4727,8 @@
       <c r="J5" t="s">
         <v>14</v>
       </c>
-      <c r="K5" t="s">
-        <v>627</v>
+      <c r="K5">
+        <v>0.8</v>
       </c>
       <c r="L5" t="s">
         <v>15</v>
@@ -4738,7 +4740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -4769,8 +4771,8 @@
       <c r="J6" t="s">
         <v>14</v>
       </c>
-      <c r="K6" t="s">
-        <v>627</v>
+      <c r="K6">
+        <v>0.8</v>
       </c>
       <c r="L6" t="s">
         <v>15</v>
@@ -4782,7 +4784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -4813,8 +4815,8 @@
       <c r="J7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" t="s">
-        <v>627</v>
+      <c r="K7">
+        <v>0.8</v>
       </c>
       <c r="L7" t="s">
         <v>15</v>
@@ -4826,7 +4828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -4857,8 +4859,8 @@
       <c r="J8" t="s">
         <v>14</v>
       </c>
-      <c r="K8" t="s">
-        <v>627</v>
+      <c r="K8">
+        <v>0.8</v>
       </c>
       <c r="L8" t="s">
         <v>15</v>
@@ -4870,7 +4872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -4901,8 +4903,8 @@
       <c r="J9" t="s">
         <v>14</v>
       </c>
-      <c r="K9" t="s">
-        <v>627</v>
+      <c r="K9">
+        <v>0.8</v>
       </c>
       <c r="L9" t="s">
         <v>15</v>
@@ -4914,7 +4916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -4945,8 +4947,8 @@
       <c r="J10" t="s">
         <v>14</v>
       </c>
-      <c r="K10" t="s">
-        <v>627</v>
+      <c r="K10">
+        <v>0.8</v>
       </c>
       <c r="L10" t="s">
         <v>15</v>
@@ -4958,7 +4960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -4989,8 +4991,8 @@
       <c r="J11" t="s">
         <v>14</v>
       </c>
-      <c r="K11" t="s">
-        <v>627</v>
+      <c r="K11">
+        <v>0.8</v>
       </c>
       <c r="L11" t="s">
         <v>15</v>
@@ -5005,7 +5007,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:N11" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:N1 A3:J11 A2:J2 L2:N2 L3:N11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -5016,9 +5018,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5080,7 +5082,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -5142,7 +5144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -5204,7 +5206,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -5266,7 +5268,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -5328,7 +5330,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -5390,7 +5392,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -5452,7 +5454,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -5514,7 +5516,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -5576,7 +5578,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5638,7 +5640,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -5714,9 +5716,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5793,7 +5795,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -5867,7 +5869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -5941,7 +5943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -6015,7 +6017,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -6089,7 +6091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -6163,7 +6165,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -6237,7 +6239,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -6311,7 +6313,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -6385,7 +6387,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -6459,7 +6461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -6547,9 +6549,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6575,7 +6577,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -6601,7 +6603,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -6627,7 +6629,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -6653,7 +6655,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -6679,7 +6681,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -6705,7 +6707,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -6731,7 +6733,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -6757,7 +6759,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -6783,7 +6785,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -6809,7 +6811,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -6849,9 +6851,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6874,7 +6876,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -6911,9 +6913,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6936,7 +6938,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -6973,9 +6975,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6989,7 +6991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -7017,9 +7019,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7054,7 +7056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -7089,7 +7091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -7124,7 +7126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -7159,7 +7161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -7194,7 +7196,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -7229,7 +7231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -7264,7 +7266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -7299,7 +7301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -7334,7 +7336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -7369,7 +7371,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -7404,7 +7406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -7439,7 +7441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -7474,7 +7476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -7509,7 +7511,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -7544,7 +7546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -7579,7 +7581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -7614,7 +7616,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -7649,7 +7651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -7684,7 +7686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -7733,9 +7735,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7794,7 +7796,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -7850,7 +7852,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -7906,7 +7908,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -7962,7 +7964,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -8018,7 +8020,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -8074,7 +8076,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -8130,7 +8132,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -8186,7 +8188,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -8242,7 +8244,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -8298,7 +8300,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -8366,11 +8368,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AS2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AP4" sqref="AP4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:45" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8507,7 +8511,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -8625,11 +8629,11 @@
       <c r="AN2" t="s">
         <v>14</v>
       </c>
-      <c r="AO2" t="s">
-        <v>390</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>390</v>
+      <c r="AO2">
+        <v>0.05</v>
+      </c>
+      <c r="AP2">
+        <v>0.05</v>
       </c>
       <c r="AQ2" t="s">
         <v>391</v>
@@ -8644,7 +8648,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:AS2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:AS1 A2:AN2 AQ2:AS2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8655,9 +8659,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8719,7 +8723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -8792,9 +8796,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8826,7 +8830,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -8858,7 +8862,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -8902,13 +8906,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8991,7 +8995,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -9065,7 +9069,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -9139,7 +9143,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -9213,7 +9217,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -9287,7 +9291,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -9361,7 +9365,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -9435,7 +9439,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -9509,7 +9513,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -9583,7 +9587,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -9657,7 +9661,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -9731,7 +9735,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -9805,7 +9809,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -9879,7 +9883,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -9953,7 +9957,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -10027,7 +10031,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -10101,7 +10105,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -10175,7 +10179,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -10249,7 +10253,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -10323,7 +10327,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -10397,7 +10401,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -10471,7 +10475,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>95</v>
       </c>
@@ -10545,7 +10549,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -10619,7 +10623,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -10693,7 +10697,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -10767,7 +10771,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -10841,7 +10845,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>115</v>
       </c>
@@ -10915,7 +10919,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>119</v>
       </c>
@@ -10989,7 +10993,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>123</v>
       </c>
@@ -11063,7 +11067,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -11137,7 +11141,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>131</v>
       </c>
@@ -11211,7 +11215,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -11285,7 +11289,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -11359,7 +11363,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -11433,7 +11437,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>148</v>
       </c>
@@ -11507,7 +11511,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>152</v>
       </c>
@@ -11581,7 +11585,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -11655,7 +11659,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -11729,7 +11733,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -11803,7 +11807,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>170</v>
       </c>
@@ -11877,7 +11881,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>174</v>
       </c>
@@ -11951,7 +11955,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>551</v>
       </c>
@@ -12025,7 +12029,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>554</v>
       </c>
@@ -12099,7 +12103,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>558</v>
       </c>
@@ -12173,7 +12177,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>561</v>
       </c>
@@ -12247,7 +12251,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>565</v>
       </c>
@@ -12321,7 +12325,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>568</v>
       </c>
@@ -12409,9 +12413,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12425,7 +12429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -12439,7 +12443,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -12467,9 +12471,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12555,7 +12559,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -12641,7 +12645,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -12727,7 +12731,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -12813,7 +12817,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -12899,7 +12903,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -12985,7 +12989,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -13071,7 +13075,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -13157,7 +13161,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -13243,7 +13247,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -13329,7 +13333,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
[WIP] tune ace data
</commit_message>
<xml_diff>
--- a/jwang/case/ieee39_ev2.xlsx
+++ b/jwang/case/ieee39_ev2.xlsx
@@ -2245,7 +2245,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L2" t="str">
         <v>1</v>
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L3" t="str">
         <v>1</v>
@@ -2333,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L4" t="str">
         <v>1</v>
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L5" t="str">
         <v>1</v>
@@ -2421,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L6" t="str">
         <v>1</v>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L7" t="str">
         <v>1</v>
@@ -2509,7 +2509,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L8" t="str">
         <v>1</v>
@@ -2553,7 +2553,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L9" t="str">
         <v>1</v>
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L10" t="str">
         <v>1</v>
@@ -2641,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="str">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L11" t="str">
         <v>1</v>
@@ -4714,7 +4714,7 @@
         <v>6</v>
       </c>
       <c r="H2" t="str">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="I2" t="str">
         <v>1.2</v>
@@ -4749,7 +4749,7 @@
         <v>4.5</v>
       </c>
       <c r="H3" t="str">
-        <v>1.84</v>
+        <v>1.2</v>
       </c>
       <c r="I3" t="str">
         <v>1.2</v>
@@ -4784,7 +4784,7 @@
         <v>2.338</v>
       </c>
       <c r="H4" t="str">
-        <v>0.84</v>
+        <v>0.6</v>
       </c>
       <c r="I4" t="str">
         <v>1.2</v>
@@ -4819,7 +4819,7 @@
         <v>5.22</v>
       </c>
       <c r="H5" t="str">
-        <v>1.766</v>
+        <v>1.2</v>
       </c>
       <c r="I5" t="str">
         <v>1.2</v>
@@ -4889,7 +4889,7 @@
         <v>3.2</v>
       </c>
       <c r="H7" t="str">
-        <v>1.53</v>
+        <v>1.4</v>
       </c>
       <c r="I7" t="str">
         <v>1.2</v>
@@ -5274,7 +5274,7 @@
         <v>2.835</v>
       </c>
       <c r="H18" t="str">
-        <v>1.269</v>
+        <v>1.1</v>
       </c>
       <c r="I18" t="str">
         <v>1.2</v>
@@ -5344,7 +5344,7 @@
         <v>4</v>
       </c>
       <c r="H20" t="str">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="I20" t="str">
         <v>1.2</v>
@@ -6259,10 +6259,10 @@
         <v>0</v>
       </c>
       <c r="AO2" t="str">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="AP2" t="str">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="AQ2" t="str">
         <v>0.1</v>

</xml_diff>

<commit_message>
Fix load and cosim
</commit_message>
<xml_diff>
--- a/jwang/case/ieee39_ev2.xlsx
+++ b/jwang/case/ieee39_ev2.xlsx
@@ -4714,7 +4714,7 @@
         <v>6</v>
       </c>
       <c r="H2" t="str">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I2" t="str">
         <v>1.2</v>
@@ -4749,7 +4749,7 @@
         <v>4.5</v>
       </c>
       <c r="H3" t="str">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I3" t="str">
         <v>1.2</v>
@@ -4819,7 +4819,7 @@
         <v>5.22</v>
       </c>
       <c r="H5" t="str">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I5" t="str">
         <v>1.2</v>
@@ -4889,7 +4889,7 @@
         <v>3.2</v>
       </c>
       <c r="H7" t="str">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="I7" t="str">
         <v>1.2</v>
@@ -5099,7 +5099,7 @@
         <v>3.086</v>
       </c>
       <c r="H13" t="str">
-        <v>-0.922</v>
+        <v>0</v>
       </c>
       <c r="I13" t="str">
         <v>1.2</v>
@@ -5912,10 +5912,10 @@
         <v>3.64</v>
       </c>
       <c r="M10" t="str">
-        <v>40</v>
+        <v>1000</v>
       </c>
       <c r="N10" t="str">
-        <v>-40</v>
+        <v>-1000</v>
       </c>
       <c r="O10" t="str">
         <v>1.052803</v>
@@ -5968,10 +5968,10 @@
         <v>-1.2</v>
       </c>
       <c r="M11" t="str">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N11" t="str">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="O11" t="str">
         <v>1.052803</v>

</xml_diff>

<commit_message>
[WIP] Fix ev_ssm control error with ict
</commit_message>
<xml_diff>
--- a/jwang/case/ieee39_ev2.xlsx
+++ b/jwang/case/ieee39_ev2.xlsx
@@ -5511,7 +5511,7 @@
         <v>6.45999998</v>
       </c>
       <c r="J3" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K3" t="str">
         <v>6.46</v>
@@ -5567,7 +5567,7 @@
         <v>7.24999998</v>
       </c>
       <c r="J4" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K4" t="str">
         <v>7.25</v>
@@ -5623,7 +5623,7 @@
         <v>6.51999998</v>
       </c>
       <c r="J5" t="str">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K5" t="str">
         <v>6.52</v>
@@ -5935,7 +5935,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="str">
         <v>PV_10</v>

</xml_diff>

<commit_message>
Fix ev_ssm control error when ict is on
</commit_message>
<xml_diff>
--- a/jwang/case/ieee39_ev2.xlsx
+++ b/jwang/case/ieee39_ev2.xlsx
@@ -5903,7 +5903,7 @@
         <v>7.64783381</v>
       </c>
       <c r="J10" t="str">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K10" t="str">
         <v>8.65</v>
@@ -5968,10 +5968,10 @@
         <v>-1.2</v>
       </c>
       <c r="M11" t="str">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="N11" t="str">
-        <v>-2000</v>
+        <v>0</v>
       </c>
       <c r="O11" t="str">
         <v>1.052803</v>

</xml_diff>